<commit_message>
update JDP | directory | Form render | create data in json (data-jdp.json) | css + html
</commit_message>
<xml_diff>
--- a/src/data/data-frm.xlsx
+++ b/src/data/data-frm.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="26">
   <si>
     <t>autonomous_community</t>
   </si>
@@ -40,10 +40,10 @@
     <t>Aragón</t>
   </si>
   <si>
-    <t>Asturias, Principado de</t>
-  </si>
-  <si>
-    <t>Baleares, Illes</t>
+    <t>Asturias</t>
+  </si>
+  <si>
+    <t>Baleares</t>
   </si>
   <si>
     <t>Canarias</t>
@@ -70,25 +70,28 @@
     <t>Galicia</t>
   </si>
   <si>
-    <t>Madrid, Comunidad de</t>
-  </si>
-  <si>
-    <t>Murcia, Región de</t>
-  </si>
-  <si>
-    <t>Navarra, Comunidad Foral de</t>
+    <t>Madrid</t>
+  </si>
+  <si>
+    <t>Murcia</t>
+  </si>
+  <si>
+    <t>Navarra</t>
   </si>
   <si>
     <t>País Vasco</t>
   </si>
   <si>
-    <t>Rioja, La</t>
+    <t>La Rioja</t>
   </si>
   <si>
     <t>Ceuta</t>
   </si>
   <si>
     <t>Melilla</t>
+  </si>
+  <si>
+    <t>ñ</t>
   </si>
 </sst>
 </file>
@@ -113,7 +116,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -521,7 +524,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -538,7 +541,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -555,7 +558,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -572,7 +575,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -589,7 +592,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -606,7 +609,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
@@ -623,7 +626,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
@@ -640,7 +643,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
@@ -657,7 +660,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
@@ -674,7 +677,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
@@ -691,7 +694,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
@@ -708,7 +711,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -725,7 +728,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
@@ -742,7 +745,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
@@ -759,7 +762,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="4" t="s">
         <v>19</v>
       </c>
@@ -776,7 +779,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
@@ -793,7 +796,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="4" t="s">
         <v>21</v>
       </c>
@@ -810,7 +813,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="4" t="s">
         <v>22</v>
       </c>
@@ -827,7 +830,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="4" t="s">
         <v>23</v>
       </c>
@@ -844,7 +847,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="4" t="s">
         <v>24</v>
       </c>
@@ -861,7 +864,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="4" t="s">
         <v>5</v>
       </c>
@@ -878,7 +881,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="4" t="s">
         <v>6</v>
       </c>
@@ -895,7 +898,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="4" t="s">
         <v>7</v>
       </c>
@@ -912,7 +915,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="4" t="s">
         <v>8</v>
       </c>
@@ -929,7 +932,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="4" t="s">
         <v>9</v>
       </c>
@@ -946,7 +949,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="4" t="s">
         <v>10</v>
       </c>
@@ -963,7 +966,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="4" t="s">
         <v>11</v>
       </c>
@@ -980,7 +983,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="4" t="s">
         <v>12</v>
       </c>
@@ -997,7 +1000,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="4" t="s">
         <v>13</v>
       </c>
@@ -1014,7 +1017,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="4" t="s">
         <v>14</v>
       </c>
@@ -1031,7 +1034,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="4" t="s">
         <v>15</v>
       </c>
@@ -1048,7 +1051,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="4" t="s">
         <v>16</v>
       </c>
@@ -1065,7 +1068,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="4" t="s">
         <v>17</v>
       </c>
@@ -1082,7 +1085,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="4" t="s">
         <v>18</v>
       </c>
@@ -1099,7 +1102,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="4" t="s">
         <v>19</v>
       </c>
@@ -1116,7 +1119,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="4" t="s">
         <v>20</v>
       </c>
@@ -1133,7 +1136,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="4" t="s">
         <v>21</v>
       </c>
@@ -1150,7 +1153,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="4" t="s">
         <v>22</v>
       </c>
@@ -1167,7 +1170,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="4" t="s">
         <v>23</v>
       </c>
@@ -1184,7 +1187,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
       <c r="A41" s="4" t="s">
         <v>24</v>
       </c>
@@ -1866,7 +1869,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="16.5">
       <c r="A81" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B81" s="5">
         <v>23.3</v>

</xml_diff>